<commit_message>
Test Case TC_001 Complete
</commit_message>
<xml_diff>
--- a/TestCase1.xlsx
+++ b/TestCase1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victorhernandez\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nagarro-my.sharepoint.com/personal/victor_hernandez_nagarro_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC34A662-D702-4226-9E3D-2864D1653E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="8_{E9FCA574-D3FA-40F8-9CC6-D5FD25BFC779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44D188E7-43BB-442D-85B4-48A3B6964F30}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AEC01738-5184-40A7-A285-433EA47F240A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="115">
   <si>
     <t>PROJECT NAME:</t>
   </si>
@@ -202,6 +202,183 @@
   </si>
   <si>
     <t>Categories were visualized in the order mentioned PHONES LAPTOPS MONITORS</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_PER_PAGE</t>
+  </si>
+  <si>
+    <t>Count of items displayed from login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login into Account </t>
+  </si>
+  <si>
+    <t>Count Items per page</t>
+  </si>
+  <si>
+    <t>9 items per page</t>
+  </si>
+  <si>
+    <t>9 Items per page</t>
+  </si>
+  <si>
+    <t>Items shown from the user´s login page</t>
+  </si>
+  <si>
+    <t>User validate the access to the account</t>
+  </si>
+  <si>
+    <t>TC_NAV_PAGES</t>
+  </si>
+  <si>
+    <t>Navigate forward &amp; Backwards from main page</t>
+  </si>
+  <si>
+    <t>Login into Account and navigate forward and backwards</t>
+  </si>
+  <si>
+    <t>Scroll down to bottom of the page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Next button </t>
+  </si>
+  <si>
+    <t>Buttons should be the only one visible and clickable</t>
+  </si>
+  <si>
+    <t>Click on next button</t>
+  </si>
+  <si>
+    <t>Next page was displayed</t>
+  </si>
+  <si>
+    <t>From second page Find Previous Button</t>
+  </si>
+  <si>
+    <t>Button should be enabled and should bring page back to initial page</t>
+  </si>
+  <si>
+    <t>When previous button was clicked page was brought back to initial page</t>
+  </si>
+  <si>
+    <t>TC_ITEM_DETAILS</t>
+  </si>
+  <si>
+    <t>Validate all 9 items from login page have details</t>
+  </si>
+  <si>
+    <t>Login into Account</t>
+  </si>
+  <si>
+    <t>Validate Item details for each item</t>
+  </si>
+  <si>
+    <t>Visual Validateion</t>
+  </si>
+  <si>
+    <t>All Items should display details of each item</t>
+  </si>
+  <si>
+    <t>All Items displayed their own decription of the item</t>
+  </si>
+  <si>
+    <t>TC_ADD_ITEMS_TO _CART</t>
+  </si>
+  <si>
+    <t>TC_DELETE_ITEMS_FROM_CART</t>
+  </si>
+  <si>
+    <t>Validate Items can be added to the cart</t>
+  </si>
+  <si>
+    <t>Login into Accont and Add Items to the cart</t>
+  </si>
+  <si>
+    <t>Select Items to add to the cart</t>
+  </si>
+  <si>
+    <t>randomly select at least 1 Items and add them to the cart</t>
+  </si>
+  <si>
+    <t>Message should be displayed "Product Added" and click OK to close the window</t>
+  </si>
+  <si>
+    <t>Message displayed"Product Added" Button OK was clicked to close the window</t>
+  </si>
+  <si>
+    <t>Validate Items can be deleted from Cart</t>
+  </si>
+  <si>
+    <t>Access Account and delete Items from Cart</t>
+  </si>
+  <si>
+    <t>From Cart delete All Items</t>
+  </si>
+  <si>
+    <t>Identify Delete option and click on all items</t>
+  </si>
+  <si>
+    <t>Each Item should be deleted when pressed the delete option</t>
+  </si>
+  <si>
+    <t>Items were deleted when delete option was clicked</t>
+  </si>
+  <si>
+    <t>TC_PLACING_AN_ORDER</t>
+  </si>
+  <si>
+    <t>Validate an order can be placed</t>
+  </si>
+  <si>
+    <t>Login into Account select items and place an order</t>
+  </si>
+  <si>
+    <t>Add Items to the Cart</t>
+  </si>
+  <si>
+    <t>Place the Order</t>
+  </si>
+  <si>
+    <t>Fill out Shipping form</t>
+  </si>
+  <si>
+    <t>Submit Order by Clicking Purchase</t>
+  </si>
+  <si>
+    <t>Closing Status order page</t>
+  </si>
+  <si>
+    <t>Select Two Items from Menu</t>
+  </si>
+  <si>
+    <t>Items should be displayed on Cart</t>
+  </si>
+  <si>
+    <t>Two Items were displayed on Cart</t>
+  </si>
+  <si>
+    <t>Shipping order form should be displayed and filled out</t>
+  </si>
+  <si>
+    <t>Shipping order form was filled out</t>
+  </si>
+  <si>
+    <t>Visual Button to be clicked</t>
+  </si>
+  <si>
+    <t>Confirmation of the Order shold be displayed with  ID, Amount, CC No. Name and date of purchase</t>
+  </si>
+  <si>
+    <t>Visual confirmation of close button</t>
+  </si>
+  <si>
+    <t>Window should close after button closed clicked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows displayed with order information </t>
+  </si>
+  <si>
+    <t>Window was closed after close button was clicked</t>
   </si>
 </sst>
 </file>
@@ -350,8 +527,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -398,6 +576,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,6 +619,25 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -753,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFEF869-2BEB-4CFC-B10A-A2BE6B67C424}">
-  <dimension ref="B2:K32"/>
+  <dimension ref="B2:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,558 +975,1248 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="21" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="2">
+      <c r="J2" s="24"/>
+      <c r="K2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="20">
+      <c r="C3" s="8"/>
+      <c r="D3" s="22">
         <v>1</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="30">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="32">
+        <v>7</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="2"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+    </row>
+    <row r="9" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K9" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14">
+    <row r="10" spans="2:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="36">
         <v>1</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G10" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="15"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
+      <c r="J10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="37"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B12" s="38"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-    </row>
-    <row r="13" spans="2:11" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="11">
+      <c r="J12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+    </row>
+    <row r="14" spans="2:11" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="12">
         <v>2</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="J14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="2:11" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-    </row>
-    <row r="17" spans="2:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14">
+      <c r="J16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:11" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+    </row>
+    <row r="18" spans="2:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="15">
         <v>3</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E18" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="J18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B19" s="16"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="17"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="26"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="3"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="3"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="18"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="3"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
+      <c r="J20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="28"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+    </row>
+    <row r="22" spans="2:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="15">
+        <v>4</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B23" s="16"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="17"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="2:11" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="28"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+    </row>
+    <row r="26" spans="2:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="15">
+        <v>5</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B27" s="16"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="16"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="17"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="28"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="2:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="15">
+        <v>6</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="20"/>
+    </row>
+    <row r="32" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B32" s="16"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="B33" s="17"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="2:11" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+    </row>
+    <row r="35" spans="2:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="12">
+        <v>7</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+    </row>
+    <row r="39" spans="2:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="12">
+        <v>8</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="2:11" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+    </row>
+    <row r="43" spans="2:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="12">
+        <v>9</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="2:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="2:11" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="39"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B9:B11"/>
+  <mergeCells count="49">
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="B43:B48"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B10:B12"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -1341,7 +2231,7 @@
     <mergeCell ref="D7:H7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G9" r:id="rId1" xr:uid="{319BDBD5-B68C-4CE8-A2BF-8169CD585E69}"/>
+    <hyperlink ref="G10" r:id="rId1" xr:uid="{319BDBD5-B68C-4CE8-A2BF-8169CD585E69}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{12621364-2360-42C1-8377-CFFBEF5B8ACE}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>